<commit_message>
updates to IRB section of paper
</commit_message>
<xml_diff>
--- a/Docs/fdt_literature.xlsx
+++ b/Docs/fdt_literature.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschap/Documents/Codes/FlowDirectionToolkit/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FA46B6-7F7B-8E44-AEE4-38185F502EBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD87A7-052B-FB4D-B617-944DE7922CA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="440" windowWidth="19820" windowHeight="20560" xr2:uid="{C56C3872-AFB7-7E4B-B5FF-96A89D5067EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$47</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -613,11 +616,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3593D92-2E2A-6845-84DB-44EB3907BD78}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,187 +653,184 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C2">
-        <v>1999</v>
+        <v>1984</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C3">
-        <v>2002</v>
+        <v>1984</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>2001</v>
+        <v>1988</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>1998</v>
+        <v>1989</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>56</v>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>2002</v>
-      </c>
-      <c r="D7" t="s">
-        <v>76</v>
+        <v>1994</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>2011</v>
+        <v>1994</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C9">
-        <v>2001</v>
+        <v>1994</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12">
-        <v>1998</v>
+        <v>1997</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>1988</v>
+        <v>1998</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>2008</v>
+        <v>1998</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -840,34 +841,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>1984</v>
+        <v>1999</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C20">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -875,71 +879,80 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>1997</v>
+        <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22">
-        <v>1984</v>
+        <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>1998</v>
+        <v>2001</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26">
-        <v>2003</v>
+        <v>2002</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -965,12 +978,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>2000</v>
+        <v>2002</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -978,10 +991,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
@@ -1009,69 +1022,66 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C31">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
       </c>
-      <c r="F31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>1994</v>
+        <v>2006</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>11</v>
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
       </c>
       <c r="C33">
-        <v>1989</v>
+        <v>2007</v>
+      </c>
+      <c r="D33" t="s">
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C34">
-        <v>2000</v>
+        <v>2008</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1</v>
-      </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C35">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1079,41 +1089,47 @@
         <v>37</v>
       </c>
       <c r="C36">
-        <v>2017</v>
+        <v>2009</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C37">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C38">
-        <v>2009</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
+        <v>2011</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1121,47 +1137,47 @@
         <v>47</v>
       </c>
       <c r="C39">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C40">
-        <v>1997</v>
-      </c>
-      <c r="D40" t="s">
-        <v>61</v>
+        <v>2013</v>
       </c>
       <c r="E40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C41">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1169,22 +1185,19 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C42">
         <v>2014</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1201,77 +1214,76 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44">
+        <v>2014</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
         <v>72</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>2016</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>70</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45">
-        <v>2013</v>
-      </c>
-      <c r="D45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C46">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C47">
-        <v>2007</v>
-      </c>
-      <c r="D47" t="s">
-        <v>77</v>
+        <v>2019</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F38">
-    <sortCondition ref="B2:B38"/>
+  <autoFilter ref="A1:F47" xr:uid="{9A4A9394-1D6B-7047-8E1A-7A1B70F303F0}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="River network upscaling"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:F47">
+    <sortCondition ref="C2:C47"/>
+    <sortCondition ref="E2:E47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>